<commit_message>
Tests working with excel data
</commit_message>
<xml_diff>
--- a/Data/AOS_DATA.xlsx
+++ b/Data/AOS_DATA.xlsx
@@ -260,7 +260,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -271,10 +271,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font/>
     <font>
@@ -387,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -407,12 +403,9 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -423,16 +416,16 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -733,8 +726,8 @@
       <c r="D2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>12</v>
+      <c r="E2" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>13</v>
@@ -757,7 +750,7 @@
       <c r="L2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="8"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
@@ -788,18 +781,18 @@
       <c r="K3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="9"/>
+      <c r="L3" s="8"/>
     </row>
     <row r="4">
-      <c r="A4" s="8"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="8"/>
       <c r="F4" s="6" t="s">
         <v>20</v>
       </c>
@@ -807,17 +800,17 @@
       <c r="H4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="9"/>
+      <c r="I4" s="8"/>
       <c r="J4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="9"/>
+      <c r="L4" s="8"/>
     </row>
     <row r="5">
-      <c r="A5" s="10"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -848,684 +841,684 @@
       <c r="K5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="9"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="13" t="s">
+      <c r="F6" s="13"/>
+      <c r="G6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="13" t="s">
+      <c r="I6" s="13"/>
+      <c r="J6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="14"/>
+      <c r="L6" s="13"/>
     </row>
     <row r="7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="13" t="s">
+      <c r="F7" s="13"/>
+      <c r="G7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="13" t="s">
+      <c r="I7" s="13"/>
+      <c r="J7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="14"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8">
-      <c r="A8" s="8"/>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="13" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="13" t="s">
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="13" t="s">
+      <c r="I8" s="13"/>
+      <c r="J8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="14"/>
+      <c r="L8" s="13"/>
     </row>
     <row r="9">
-      <c r="A9" s="10"/>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="13" t="s">
+      <c r="F9" s="13"/>
+      <c r="G9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="13" t="s">
+      <c r="I9" s="13"/>
+      <c r="J9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="14"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="10">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="17" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
     </row>
     <row r="11">
-      <c r="A11" s="8"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
     </row>
     <row r="12">
-      <c r="A12" s="8"/>
-      <c r="B12" s="18" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
     </row>
     <row r="13">
-      <c r="A13" s="10"/>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
     </row>
     <row r="14">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22" t="s">
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="L14" s="22" t="s">
+      <c r="L14" s="21" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="10"/>
-      <c r="B15" s="20" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="L15" s="22" t="s">
+      <c r="L15" s="21" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="26" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="K16" s="26" t="s">
+      <c r="K16" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="L16" s="26" t="s">
+      <c r="L16" s="25" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="8"/>
-      <c r="B17" s="24" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="27" t="s">
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="27" t="s">
+      <c r="K17" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="L17" s="27" t="s">
+      <c r="L17" s="26" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="8"/>
-      <c r="B18" s="24" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="26" t="s">
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="K18" s="26" t="s">
+      <c r="K18" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="L18" s="26" t="s">
+      <c r="L18" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="8"/>
-      <c r="B19" s="28" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="26" t="s">
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="K19" s="26" t="s">
+      <c r="K19" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="L19" s="26" t="s">
+      <c r="L19" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="8"/>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="26" t="s">
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="K20" s="26" t="s">
+      <c r="K20" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="L20" s="26" t="s">
+      <c r="L20" s="25" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="8"/>
-      <c r="B21" s="24" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="26" t="s">
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="K21" s="26" t="s">
+      <c r="K21" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="L21" s="26" t="s">
+      <c r="L21" s="25" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="8"/>
-      <c r="B22" s="24" t="s">
+      <c r="A22" s="7"/>
+      <c r="B22" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="26" t="s">
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="K22" s="26" t="s">
+      <c r="K22" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="L22" s="26" t="s">
+      <c r="L22" s="25" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="8"/>
-      <c r="B23" s="24" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="26" t="s">
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="K23" s="26" t="s">
+      <c r="K23" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="L23" s="26" t="s">
+      <c r="L23" s="25" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="8"/>
-      <c r="B24" s="24" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="26" t="s">
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="K24" s="26" t="s">
+      <c r="K24" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="L24" s="26" t="s">
+      <c r="L24" s="25" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="24" t="s">
+      <c r="A25" s="7"/>
+      <c r="B25" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="26" t="s">
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="K25" s="26" t="s">
+      <c r="K25" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="L25" s="26" t="s">
+      <c r="L25" s="25" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="8"/>
-      <c r="B26" s="24" t="s">
+      <c r="A26" s="7"/>
+      <c r="B26" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="26" t="s">
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="K26" s="26" t="s">
+      <c r="K26" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="L26" s="26" t="s">
+      <c r="L26" s="25" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="10"/>
-      <c r="B27" s="24" t="s">
+      <c r="A27" s="9"/>
+      <c r="B27" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="26" t="s">
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="K27" s="26" t="s">
+      <c r="K27" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="L27" s="26" t="s">
+      <c r="L27" s="25" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="13" t="s">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="K28" s="13"/>
-      <c r="L28" s="14"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="13"/>
     </row>
     <row r="29">
-      <c r="A29" s="10"/>
-      <c r="B29" s="12" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="13" t="s">
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="K29" s="13"/>
-      <c r="L29" s="14"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="13"/>
     </row>
     <row r="30">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="27" t="s">
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="L30" s="25"/>
+      <c r="L30" s="24"/>
     </row>
     <row r="31">
-      <c r="A31" s="8"/>
-      <c r="B31" s="24" t="s">
+      <c r="A31" s="7"/>
+      <c r="B31" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="26" t="s">
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="L31" s="25"/>
+      <c r="L31" s="24"/>
     </row>
     <row r="32">
-      <c r="A32" s="8"/>
-      <c r="B32" s="24" t="s">
+      <c r="A32" s="7"/>
+      <c r="B32" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="26" t="s">
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="L32" s="25"/>
+      <c r="L32" s="24"/>
     </row>
     <row r="33">
-      <c r="A33" s="8"/>
-      <c r="B33" s="24" t="s">
+      <c r="A33" s="7"/>
+      <c r="B33" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="26" t="s">
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="L33" s="25"/>
+      <c r="L33" s="24"/>
     </row>
     <row r="34">
-      <c r="A34" s="10"/>
-      <c r="B34" s="24" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="26" t="s">
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="L34" s="25"/>
+      <c r="L34" s="24"/>
     </row>
     <row r="35">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="29" t="s">
         <v>80</v>
       </c>
       <c r="B35" s="1"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="30"/>
     </row>
     <row r="36">
-      <c r="L36" s="32"/>
+      <c r="L36" s="31"/>
     </row>
     <row r="37">
-      <c r="L37" s="32"/>
+      <c r="L37" s="31"/>
     </row>
     <row r="38">
-      <c r="L38" s="32"/>
+      <c r="L38" s="31"/>
     </row>
     <row r="39">
-      <c r="L39" s="32"/>
+      <c r="L39" s="31"/>
     </row>
     <row r="40">
-      <c r="L40" s="32"/>
+      <c r="L40" s="31"/>
     </row>
     <row r="41">
-      <c r="L41" s="32"/>
+      <c r="L41" s="31"/>
     </row>
     <row r="42">
-      <c r="L42" s="32"/>
+      <c r="L42" s="31"/>
     </row>
     <row r="43">
-      <c r="L43" s="32"/>
+      <c r="L43" s="31"/>
     </row>
     <row r="44">
-      <c r="L44" s="32"/>
+      <c r="L44" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Add description to ecxel
</commit_message>
<xml_diff>
--- a/Data/AOS_DATA.xlsx
+++ b/Data/AOS_DATA.xlsx
@@ -1639,14 +1639,46 @@
           <t>X</t>
         </is>
       </c>
-      <c r="E35" s="30" t="n"/>
-      <c r="F35" s="30" t="n"/>
-      <c r="G35" s="30" t="n"/>
-      <c r="H35" s="30" t="n"/>
-      <c r="I35" s="30" t="n"/>
-      <c r="J35" s="30" t="n"/>
-      <c r="K35" s="30" t="n"/>
-      <c r="L35" s="30" t="n"/>
+      <c r="E35" s="30" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="F35" s="30" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="G35" s="30" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="H35" s="30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I35" s="30" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="J35" s="30" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="K35" s="30" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="L35" s="30" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="L36" s="31" t="n"/>

</xml_diff>